<commit_message>
add weekly group meeting instance
</commit_message>
<xml_diff>
--- a/documentation/GroupProjectPlan.xlsx
+++ b/documentation/GroupProjectPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>Task</t>
   </si>
@@ -37,19 +37,25 @@
     <t>Actual Effort (hours)</t>
   </si>
   <si>
+    <t>Weekly Group Meeting - Discuss development plan</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
     <t>Hardware Testing - Voice and Sound IO</t>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>In-class</t>
   </si>
   <si>
     <t>Set up Github repository</t>
   </si>
   <si>
-    <t>Link GTTS (Google Text to Speech) to System</t>
+    <t>Figure out GTTS (Google Text to Speech)</t>
   </si>
   <si>
     <t/>
@@ -498,13 +504,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="6">
-        <v>44967</v>
+        <v>44965</v>
       </c>
       <c r="E2" s="5">
         <v>100</v>
       </c>
       <c r="F2" s="6">
-        <v>44967</v>
+        <v>44965</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>9</v>
@@ -518,7 +524,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6">
         <v>44967</v>
@@ -530,18 +536,18 @@
         <v>44967</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="6">
         <v>44967</v>
@@ -553,67 +559,81 @@
         <v>44967</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6">
+        <v>44967</v>
+      </c>
+      <c r="E5" s="5">
+        <v>100</v>
+      </c>
+      <c r="F5" s="6">
+        <v>44967</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
       <c r="F6" s="4"/>
       <c r="G6" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
       <c r="F7" s="4"/>
       <c r="G7" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
       <c r="F8" s="4"/>
       <c r="G8" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">

</xml_diff>

<commit_message>
added next week's plans
</commit_message>
<xml_diff>
--- a/documentation/GroupProjectPlan.xlsx
+++ b/documentation/GroupProjectPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jneal\Desktop\Internet of Things\CPSC-341-01-S23-Twister\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D1CFC9-3302-4FC7-81AA-FF27AF1E7C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E74973E-D513-409B-9F98-65A5951DE4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Find module to do input</t>
+  </si>
+  <si>
+    <t>~ 3 hours</t>
   </si>
 </sst>
 </file>
@@ -777,7 +780,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +824,9 @@
       <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D2" s="6">
         <v>44972</v>
       </c>
@@ -857,7 +862,9 @@
       <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D4" s="6">
         <v>44972</v>
       </c>

</xml_diff>